<commit_message>
example for scraping and crawling
</commit_message>
<xml_diff>
--- a/links.xlsx
+++ b/links.xlsx
@@ -375,195 +375,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Apple iPhone XR (64GB) - Blue</v>
+        <v>Name</v>
       </c>
       <c r="B1" t="str">
-        <v>Apple iPhone 11 (128GB) - Black</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Vivo U10 (Electric Blue, 5000 mAH 18W Fast Charge Battery, 3GB RAM, 32GB Storage)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>OPPO A1K (Black, 2GB RAM, 32GB Storage) with No Cost EMI/Additional Exchange Offers</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Samsung Galaxy M21 (Midnight Blue, 4GB RAM, 64GB Storage)</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Vivo U20 (Blazing Blue, Snapdragon 675 AIE, 4GB RAM, 64GB Storage)</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Samsung Galaxy M31 (Ocean Blue, 6GB RAM, 64GB Storage)</v>
-      </c>
-      <c r="H1" t="str">
-        <v>IKall K8 Smartphone (5.5 Inch, 16GB) (Red)</v>
-      </c>
-      <c r="I1" t="str">
-        <v>itel A46 (Neon Water, 2GB RAM, 16GB Storage)</v>
-      </c>
-      <c r="J1" t="str">
-        <v>Vivo Y91i (Fusion Black, 2GB RAM, 32GB Storage) with No Cost EMI/Additional Exchange Offers</v>
-      </c>
-      <c r="K1" t="str">
-        <v>Redmi 7A (Matte Blue, 2GB RAM, 16GB Storage)</v>
-      </c>
-      <c r="L1" t="str">
-        <v>Vivo Y91i (Ocean Blue, 2GB RAM, 32GB Storage) with No Cost EMI/Additional Exchange Offers</v>
-      </c>
-      <c r="M1" t="str">
-        <v>Redmi 8A Dual (Sea Blue, 2GB RAM, 32GB Storage) – Dual Cameras &amp; 5,000 mAH Battery</v>
-      </c>
-      <c r="N1" t="str">
-        <v>Samsung Galaxy M21 (Raven Black, 4GB RAM, 64GB Storage)</v>
-      </c>
-      <c r="O1" t="str">
-        <v>Mi 10 (Twilight Grey, 8GB RAM, 128GB Storage) - 108MP Quad Camera, SD 865 Processor, 5G Ready</v>
-      </c>
-      <c r="P1" t="str">
-        <v>Sharp Icon Fancy Printed Designer Leather Flip Wallet Back Cover Case for Samsung Galaxy A7 2018</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>OPPO A1K (Red, 2GB RAM, 32GB Storage) with No Cost EMI/Additional Exchange Offers</v>
-      </c>
-      <c r="R1" t="str">
-        <v>Redmi 8A Dual (Sky White, 2GB RAM, 32GB Storage) – Dual Cameras &amp; 5,000 mAH Battery</v>
-      </c>
-      <c r="S1" t="str">
-        <v>OPPO A11K (Flowing Silver, 2GB RAM, 32GB Storage) with No Cost EMI/Additional Exchange Offers</v>
-      </c>
-      <c r="T1" t="str">
-        <v>Samsung Galaxy M31 (Space Black, 6GB RAM, 128GB Storage)</v>
-      </c>
-      <c r="U1" t="str">
-        <v>Samsung Galaxy M21 (Raven Black, 6GB RAM, 128GB Storage)</v>
-      </c>
-      <c r="V1" t="str">
-        <v>Vivo U10 (Thunder Black, 5000 mAH 18W Fast Charge Battery, 3GB RAM, 64GB Storage)</v>
-      </c>
-      <c r="W1" t="str">
-        <v>IKall K4 Android Mobile (2GB, 16GB)</v>
-      </c>
-      <c r="X1" t="str">
-        <v>Samsung Galaxy M30s (Opal Black, 4GB RAM, 64GB Storage)</v>
-      </c>
-      <c r="Y1" t="str">
-        <v>Samsung Galaxy M30 (Gradation Blue, 4GB RAM, Super AMOLED Display, 64GB Storage, 5000mAH Battery)</v>
-      </c>
-      <c r="Z1" t="str">
-        <v>ELV 4mm Thickness Aluminum mobile Stand (3.5 - 8 inches) - Black</v>
-      </c>
-      <c r="AA1" t="str">
-        <v>Vivo Y30 (Emerald Black, 4GB RAM, 128GB Storage) with No Cost EMI/Additional Exchange Offers</v>
-      </c>
-      <c r="AB1" t="str">
-        <v>OPPO A31 (Fantasy White, 4GB RAM, 64GB Storage) with No Cost EMI/Additional Exchange Offers</v>
-      </c>
-      <c r="AC1" t="str">
-        <v>Sharp Icon Fancy Printed Designer Leather Flip Wallet Back Cover Case for Samsung Galaxy J6</v>
-      </c>
-      <c r="AD1" t="str">
-        <v>Sharp Icon Fancy Printed Designer Leather Flip Wallet Back Cover Case for Samsung Galaxy J8</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>52,500</v>
-      </c>
-      <c r="B2" t="str">
-        <v>73,600</v>
-      </c>
-      <c r="C2" t="str">
-        <v>10,990</v>
-      </c>
-      <c r="D2" t="str">
-        <v>7,990</v>
-      </c>
-      <c r="E2" t="str">
-        <v>13,999</v>
-      </c>
-      <c r="F2" t="str">
-        <v>12,990</v>
-      </c>
-      <c r="G2" t="str">
-        <v>16,499</v>
-      </c>
-      <c r="H2" t="str">
-        <v>4,899</v>
-      </c>
-      <c r="I2" t="str">
-        <v>7,990</v>
-      </c>
-      <c r="J2" t="str">
-        <v>5,999</v>
-      </c>
-      <c r="K2" t="str">
-        <v>7,990</v>
-      </c>
-      <c r="L2" t="str">
-        <v>7,499</v>
-      </c>
-      <c r="M2" t="str">
-        <v>13,999</v>
-      </c>
-      <c r="N2" t="str">
-        <v>49,999</v>
-      </c>
-      <c r="O2" t="str">
-        <v>599</v>
-      </c>
-      <c r="P2" t="str">
-        <v>7,990</v>
-      </c>
-      <c r="Q2" t="str">
-        <v>7,499</v>
-      </c>
-      <c r="R2" t="str">
-        <v>8,990</v>
-      </c>
-      <c r="S2" t="str">
-        <v>17,499</v>
-      </c>
-      <c r="T2" t="str">
-        <v>15,999</v>
-      </c>
-      <c r="U2" t="str">
-        <v>11,490</v>
-      </c>
-      <c r="V2" t="str">
-        <v>5,099</v>
-      </c>
-      <c r="W2" t="str">
-        <v>14,999</v>
-      </c>
-      <c r="X2" t="str">
-        <v>12,999</v>
-      </c>
-      <c r="Y2" t="str">
-        <v>149</v>
-      </c>
-      <c r="Z2" t="str">
-        <v>14,990</v>
-      </c>
-      <c r="AA2" t="str">
-        <v>12,490</v>
-      </c>
-      <c r="AB2" t="str">
-        <v>599</v>
-      </c>
-      <c r="AC2" t="str">
-        <v>599</v>
+        <v>Price</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AD2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fetch data from web store in xlsx
</commit_message>
<xml_diff>
--- a/links.xlsx
+++ b/links.xlsx
@@ -375,22 +375,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Name</v>
+        <v>Apple iPhone 7 (32GB) - Black</v>
       </c>
       <c r="B1" t="str">
-        <v>Price</v>
+        <v>Apple iPhone 11 (128GB) - Black</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Vivo U10 (Electric Blue, 5000 mAH 18W Fast Charge Battery, 3GB RAM, 32GB Storage)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Nokia 105 2019 (Single SIM, Black)</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Samsung Galaxy M21 (Midnight Blue, 4GB RAM, 64GB Storage)</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Samsung Galaxy M31 (Ocean Blue, 6GB RAM, 128GB Storage)</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Vivo Y91i (Fusion Black, 2GB RAM, 32GB Storage) with No Cost EMI/Additional Exchange Offers</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Redmi Note 8 Pro (Halo White, 6GB RAM, 128GB Storage with Helio G90T Processor)</v>
+      </c>
+      <c r="I1" t="str">
+        <v>SNEXIAN Guru 106 Dual Sim Basic Mobile Phone with Digital Camera and 1.8 inch Screen (Black, Upto 16GB) - NO Charger</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Vivo Y91i (Ocean Blue, 2GB RAM, 32GB Storage) with No Cost EMI/Additional Exchange Offers</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Karbonn KX3 1.8 inch Display Feature Phone with Bluetooth,Dual Sim, 0.3 MP Digital Camera with Zoom, 800 mAH Battery,32 GB Expandable Memory and Support for MP3+MP4, Boom Box Speaker,Black Red Colour.</v>
+      </c>
+      <c r="L1" t="str">
+        <v>itel A46 (Neon Water, 2GB RAM, 16GB Storage)</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Samsung Galaxy M21 (Raven Black, 6GB RAM, 128GB Storage)</v>
+      </c>
+      <c r="N1" t="str">
+        <v>SNEXIAN Guru 311 Dual Sim Basic Mobile Phone with Digital Camera and 1.8 inch Screen (Black, Upto 16GB) - NO Charger</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Maono AU-D30 BassCurve Neck Band in-Ear Bluetooth Wireless Earphones, with Bluetooth 5.0, Sweatproof Headphones, Long Life Battery, Flexible Headset and Built-in Mic</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Spigen [Rugged Armor] Case for Huawei P30, Patent Design Flexible TPU Phone Case Cover for Huawei P30 (NOT Compatible with P30 Pro / P30 Lite)</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>TECNO Spark 5 Pro (Seabed Blue, 4GB RAM, 64GB Storage)</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Nokia 105 2019 (Single SIM, Blue)</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Nokia 105 2019 (Single SIM, Pink)</v>
+      </c>
+      <c r="T1" t="str">
+        <v>ELV 4mm Thickness Aluminum mobile Stand (3.5 - 8 inches) - Black</v>
+      </c>
+      <c r="U1" t="str">
+        <v>IKall K76 Mobile (1.4 Inch Display, Single Sim, 600 mAh Battery) (Yellow)</v>
+      </c>
+      <c r="V1" t="str">
+        <v>Samsung Galaxy M21 (Raven Black, 4GB RAM, 64GB Storage)</v>
+      </c>
+      <c r="W1" t="str">
+        <v>OPPO A5 2020 (Dazzling White, 3GB RAM, 64GB Storage) with No Cost EMI/Additional Exchange Offers</v>
+      </c>
+      <c r="X1" t="str">
+        <v>OPPO F11 (Fluorite Purple, 6GB RAM, 128GB Storage) with No Cost EMI/Additional Exchange Offers</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>OPPO A5 2020 (Dazzling White, 4GB RAM, 64GB Storage) with No Cost EMI/Additional Exchange Offers</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>Vivo U10 (Thunder Black,5000 mAH 18W Fast Charge Battery, 3GB RAM, 32GB Storage)</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>Micromax X421 Black</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>Redmi 8A Dual (Sky White, 2GB RAM, 32GB Storage) – Dual Cameras &amp; 5,000 mAH Battery</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>Lenovo HT10 True Wireless Earbuds Earphones Headphones (Bluetooth V5.0) in-Built Mic with Extra HD Sound AirBass Rated IPX5 Waterproof and Sweatproof (Black)</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>Spigen Slim Armor CS Flip Wallet Card Slot Holder Back Cover Case Designed for iPhone 11 - Gunmetal</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>29,499</v>
+      </c>
+      <c r="B2" t="str">
+        <v>73,600</v>
+      </c>
+      <c r="C2" t="str">
+        <v>10,990</v>
+      </c>
+      <c r="D2" t="str">
+        <v>1,241</v>
+      </c>
+      <c r="E2" t="str">
+        <v>13,999</v>
+      </c>
+      <c r="F2" t="str">
+        <v>17,499</v>
+      </c>
+      <c r="G2" t="str">
+        <v>7,990</v>
+      </c>
+      <c r="H2" t="str">
+        <v>16,999</v>
+      </c>
+      <c r="I2" t="str">
+        <v>599</v>
+      </c>
+      <c r="J2" t="str">
+        <v>7,990</v>
+      </c>
+      <c r="K2" t="str">
+        <v>805</v>
+      </c>
+      <c r="L2" t="str">
+        <v>15,999</v>
+      </c>
+      <c r="M2" t="str">
+        <v>599</v>
+      </c>
+      <c r="N2" t="str">
+        <v>1,299</v>
+      </c>
+      <c r="O2" t="str">
+        <v>899</v>
+      </c>
+      <c r="P2" t="str">
+        <v>10,499</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>1,105</v>
+      </c>
+      <c r="R2" t="str">
+        <v>1,230</v>
+      </c>
+      <c r="S2" t="str">
+        <v>149</v>
+      </c>
+      <c r="T2" t="str">
+        <v>399</v>
+      </c>
+      <c r="U2" t="str">
+        <v>13,999</v>
+      </c>
+      <c r="V2" t="str">
+        <v>10,990</v>
+      </c>
+      <c r="W2" t="str">
+        <v>18,990</v>
+      </c>
+      <c r="X2" t="str">
+        <v>11,990</v>
+      </c>
+      <c r="Y2" t="str">
+        <v>10,990</v>
+      </c>
+      <c r="Z2" t="str">
+        <v>1,020</v>
+      </c>
+      <c r="AA2" t="str">
+        <v>7,499</v>
+      </c>
+      <c r="AB2" t="str">
+        <v>3,999</v>
+      </c>
+      <c r="AC2" t="str">
+        <v>1,599</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AD2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>